<commit_message>
hopefully final commit, integrated matrix ops
</commit_message>
<xml_diff>
--- a/src/tests/sheet1.xlsx
+++ b/src/tests/sheet1.xlsx
@@ -111,13 +111,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C3"/>
+  <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -126,21 +126,11 @@
       <c r="C1" s="0" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="n">
-        <v>3</v>
+      <c r="D1" s="0" t="n">
+        <v>4.4</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
-        <v>3.55</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>233.006</v>
+      <c r="E1" s="0" t="n">
+        <v>1231.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>